<commit_message>
added comments, top is tracked by text
</commit_message>
<xml_diff>
--- a/documentation/project3_hours.xlsx
+++ b/documentation/project3_hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/landen/Desktop/Classes/Spring22/eecs448/Project3/ds_visualizer/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duy Vu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3AC450-05C9-FB40-B998-A8EEA2EAA44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6955C0E4-1598-4BDF-B5EA-6563619D7154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35240" yWindow="640" windowWidth="28040" windowHeight="16940" xr2:uid="{095FDC74-654F-AD46-9E96-47D17C496F71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{095FDC74-654F-AD46-9E96-47D17C496F71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>Hour Tracking - Project 3</t>
+  </si>
+  <si>
+    <t>Duy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duy </t>
   </si>
 </sst>
 </file>
@@ -95,10 +101,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,19 +422,19 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -439,61 +445,77 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>44641</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44646</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44650</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated Hours - Eric
</commit_message>
<xml_diff>
--- a/documentation/project3_hours.xlsx
+++ b/documentation/project3_hours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duy Vu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Z\Desktop\Battleship Game Project 1 EECS448\Project 3\ds_visualizer\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6955C0E4-1598-4BDF-B5EA-6563619D7154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E43A8C-140F-49B0-9D87-4D08893AB7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{095FDC74-654F-AD46-9E96-47D17C496F71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{095FDC74-654F-AD46-9E96-47D17C496F71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -56,6 +55,12 @@
   </si>
   <si>
     <t xml:space="preserve">Duy </t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eric </t>
   </si>
 </sst>
 </file>
@@ -419,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C9284C-DDD1-9340-9499-ED661EE2284D}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -469,26 +474,58 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44647</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44648</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44649</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44650</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B9" s="1">
         <v>44650</v>
       </c>
-      <c r="C5">
+      <c r="C9">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
@@ -516,6 +553,12 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added total counter to hours
</commit_message>
<xml_diff>
--- a/documentation/project3_hours.xlsx
+++ b/documentation/project3_hours.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Z\Desktop\Battleship Game Project 1 EECS448\Project 3\ds_visualizer\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E43A8C-140F-49B0-9D87-4D08893AB7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820CBD7A-8F94-43DB-944E-55CEA891A1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{095FDC74-654F-AD46-9E96-47D17C496F71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t xml:space="preserve">Eric </t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -104,12 +107,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +431,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -548,16 +552,23 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f>SUM(C3:C16)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
   </sheetData>
@@ -565,5 +576,6 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating hours pt. 2
</commit_message>
<xml_diff>
--- a/documentation/project3_hours.xlsx
+++ b/documentation/project3_hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/landen/Desktop/Classes/Spring22/eecs448/Project3/ds_visualizer/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1CF2F2-2EF4-5844-A9D1-C2E05C89AA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A294CC7-FAB2-7045-B7A0-C7E38C2A009D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="500" windowWidth="27720" windowHeight="15840" xr2:uid="{095FDC74-654F-AD46-9E96-47D17C496F71}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>